<commit_message>
Updating Old File for core commit 7ea7761f573aaeb3a9bc47f1d15071898a3d724e
</commit_message>
<xml_diff>
--- a/help/dev/before-implement/assets/FPC_Request_Form.xlsx
+++ b/help/dev/before-implement/assets/FPC_Request_Form.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfrei\Documents\Git\target-dev.en\help\dev\before-implement\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CC57DD-1919-4561-B84E-979D02F4E117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-5820" windowWidth="51200" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPC Request Form" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Aaron Hadley</author>
   </authors>
   <commentList>
-    <comment ref="J11" authorId="0">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0">
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -66,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0">
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0">
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -92,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="0">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0">
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0">
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J21" authorId="0">
+    <comment ref="J21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -147,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0">
+    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J23" authorId="0">
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -180,18 +186,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>First Party Cookie (CNAME):  Request Form</t>
   </si>
   <si>
     <t>Fill in all required fields in the form below (see sample for reference)</t>
-  </si>
-  <si>
-    <t>Forward this request form to clientcare@adobe.com</t>
-  </si>
-  <si>
-    <t>Update CNAMEs to point to Adobe Hostnames that will be provided by Client Care</t>
   </si>
   <si>
     <t>Adobe purchases and applies certificate during the next available maintenance window</t>
@@ -324,23 +324,69 @@
     <t>Certificate Management</t>
   </si>
   <si>
-    <t>Adobe will purchase and maintain your certificate during each subsequent renewal cycle.  Exemptions to the Adobe Managed Certificate Program can be submitted to clientcare@adobe.com for consideration and approval.</t>
-  </si>
-  <si>
     <t>Regional Data Collection (RDC)</t>
   </si>
   <si>
-    <t>https://marketing.adobe.com/resources/help/en_US/whitepapers/rdc/</t>
-  </si>
-  <si>
-    <t>Adobe Regional Data Collection (RDC) is a network of regional data collection centers that aim to reduce latency and data loss associated with Adobe image requests.  All new CNAME implementations will be configured for RDC.  More information can be found here</t>
+    <t>Update CNAMEs to point to Adobe Hostnames that will be provided by Adobe</t>
+  </si>
+  <si>
+    <t>Adobe will purchase and maintain your certificate during each subsequent renewal cycle.  Exemptions to the Adobe Managed Certificate Program can be submitted to Adobe for consideration and approval.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adobe Regional Data Collection (RDC) is a network of regional data collection centers that aim to reduce latency and data loss associated with Adobe image requests.  All new CNAME implementations will be configured for RDC.  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a Support case in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Admin Console</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Support </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and attach the file to that ticket</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -416,6 +462,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -618,9 +679,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -630,15 +691,117 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,122 +817,23 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -783,6 +847,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1107,14 +1179,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="2" width="4.33203125" customWidth="1"/>
     <col min="3" max="5" width="15.83203125" customWidth="1"/>
@@ -1122,24 +1194,24 @@
     <col min="12" max="13" width="4.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:15" ht="23.35" x14ac:dyDescent="0.8">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
-    </row>
-    <row r="2" spans="1:15" ht="18">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="55"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1154,100 +1226,100 @@
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="18">
+    <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A3" s="6"/>
-      <c r="B3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="16"/>
+      <c r="B3" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="50"/>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="18">
+    <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A4" s="6"/>
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="18"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="52"/>
       <c r="M4" s="8"/>
     </row>
-    <row r="5" spans="1:15" ht="18">
+    <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A5" s="6"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="20"/>
+      <c r="C5" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="44"/>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:15" ht="18">
+    <row r="6" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A6" s="6"/>
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
+      <c r="C6" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="44"/>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:15" ht="18">
+    <row r="7" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A7" s="6"/>
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
+      <c r="C7" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
+      <c r="H7" s="45"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="45"/>
+      <c r="L7" s="46"/>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" ht="18">
+    <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1262,290 +1334,290 @@
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:15" ht="18">
+    <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="C9" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="7"/>
-      <c r="J9" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="28"/>
+      <c r="J9" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="25"/>
       <c r="L9" s="5"/>
       <c r="M9" s="9"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="18">
+    <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
+      <c r="C10" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="42"/>
       <c r="L10" s="5"/>
       <c r="M10" s="9"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="18">
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
+      <c r="C11" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="21"/>
+      <c r="J11" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="26"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:15" ht="18">
+    <row r="12" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="C12" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="21"/>
+      <c r="J12" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="26"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:15" ht="18">
+    <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
+      <c r="C13" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="21"/>
+      <c r="J13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="26"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:15" ht="18">
+    <row r="14" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="7"/>
-      <c r="J14" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="21"/>
+      <c r="J14" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="26"/>
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:15" ht="18">
+    <row r="15" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
       <c r="I15" s="7"/>
-      <c r="J15" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="21"/>
+      <c r="J15" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="26"/>
       <c r="L15" s="7"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:15" ht="18">
+    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.6">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
+      <c r="C16" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
       <c r="I16" s="7"/>
-      <c r="J16" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="21"/>
+      <c r="J16" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="26"/>
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
     </row>
-    <row r="17" spans="1:13" ht="18">
+    <row r="17" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
+      <c r="C17" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" ht="18">
+    <row r="18" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
+      <c r="C18" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="21"/>
+      <c r="J18" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="26"/>
       <c r="L18" s="7"/>
       <c r="M18" s="8"/>
     </row>
-    <row r="19" spans="1:13" ht="18">
+    <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="C19" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="43">
+      <c r="J19" s="27">
         <v>10000</v>
       </c>
-      <c r="K19" s="21"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
     </row>
-    <row r="20" spans="1:13" ht="18">
+    <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
+      <c r="C20" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
       <c r="I20" s="7"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
       <c r="L20" s="7"/>
       <c r="M20" s="8"/>
     </row>
-    <row r="21" spans="1:13" ht="18">
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="45" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="C21" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K21" s="21"/>
+      <c r="J21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="26"/>
       <c r="L21" s="7"/>
       <c r="M21" s="8"/>
     </row>
-    <row r="22" spans="1:13" ht="18">
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
+      <c r="C22" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="7"/>
-      <c r="J22" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="21"/>
+      <c r="J22" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="26"/>
       <c r="L22" s="7"/>
       <c r="M22" s="8"/>
     </row>
-    <row r="23" spans="1:13" ht="18">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
+      <c r="C23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="21"/>
+      <c r="J23" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="26"/>
       <c r="L23" s="7"/>
       <c r="M23" s="8"/>
     </row>
-    <row r="24" spans="1:13" ht="18">
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1560,79 +1632,77 @@
       <c r="L24" s="7"/>
       <c r="M24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="18">
+    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.6">
       <c r="A25" s="6"/>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" ht="58" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A26" s="6"/>
+      <c r="B26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" ht="93" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A27" s="6"/>
+      <c r="B27" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="8"/>
-    </row>
-    <row r="26" spans="1:13" ht="58" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="8"/>
-    </row>
-    <row r="27" spans="1:13" ht="93" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="47" t="s">
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="52"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="19"/>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="1:13" ht="18">
+    <row r="28" spans="1:13" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="10"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="53" t="s">
-        <v>36</v>
-      </c>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="55"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -1649,12 +1719,38 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="E27:L27"/>
-    <mergeCell ref="E28:L28"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="C5:L5"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C6:L6"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J14:K14"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="J18:K18"/>
     <mergeCell ref="J19:K19"/>
@@ -1671,45 +1767,18 @@
     <mergeCell ref="F23:H23"/>
     <mergeCell ref="C19:E19"/>
     <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C17:H17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C6:L6"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="E28:L28"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J16" r:id="rId1"/>
-    <hyperlink ref="E28" r:id="rId2"/>
+    <hyperlink ref="J16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>